<commit_message>
30 removed the picture link from the Excel file. and commented // the step under addemployeesteps. will run without until we find a solution
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/EmployeesExcel.xlsx
+++ b/src/test/resources/testdata/EmployeesExcel.xlsx
@@ -65,7 +65,7 @@
     <t>jgjguk14dp3</t>
   </si>
   <si>
-    <t>xcGzvc1241</t>
+    <t>xcGzRvc12412</t>
   </si>
 </sst>
 </file>
@@ -73,10 +73,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -94,6 +94,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -101,25 +109,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -148,23 +169,46 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -178,61 +222,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,13 +253,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -271,55 +403,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -337,103 +427,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -449,11 +449,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -512,24 +510,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -544,153 +524,173 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1120,7 +1120,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
Executing the project in Jenkins
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/EmployeesExcel.xlsx
+++ b/src/test/resources/testdata/EmployeesExcel.xlsx
@@ -65,7 +65,7 @@
     <t>jgjguk14dp3</t>
   </si>
   <si>
-    <t>xcGzRvc1q</t>
+    <t>xcGzRvc1ql</t>
   </si>
 </sst>
 </file>
@@ -73,10 +73,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -95,6 +95,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -102,7 +109,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -118,7 +140,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -126,37 +148,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -171,6 +163,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -185,6 +184,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -203,6 +216,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -212,27 +233,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,12 +253,72 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -271,13 +331,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,151 +433,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -447,32 +447,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -516,11 +495,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -535,21 +544,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -567,130 +567,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>

</xml_diff>

<commit_message>
Executing the project in Jenkins smoke and regression.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/EmployeesExcel.xlsx
+++ b/src/test/resources/testdata/EmployeesExcel.xlsx
@@ -65,7 +65,7 @@
     <t>jgjguk14dp3</t>
   </si>
   <si>
-    <t>xcGzRvc1ql</t>
+    <t>xcGzRvfc12qly</t>
   </si>
 </sst>
 </file>
@@ -73,10 +73,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -94,8 +94,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -108,23 +116,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -132,23 +126,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -162,20 +140,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -185,14 +149,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -216,6 +173,35 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -224,15 +210,29 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,13 +253,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -271,169 +415,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -447,11 +447,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -480,17 +486,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -513,8 +513,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -549,148 +549,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>

</xml_diff>

<commit_message>
Executing the project in Jenkins smoke and regression.2
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/EmployeesExcel.xlsx
+++ b/src/test/resources/testdata/EmployeesExcel.xlsx
@@ -65,7 +65,7 @@
     <t>jgjguk14dp3</t>
   </si>
   <si>
-    <t>jhvjvjvhhv</t>
+    <t>jh2vjvjdockers</t>
   </si>
 </sst>
 </file>
@@ -73,10 +73,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -103,45 +103,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -155,6 +132,82 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -163,76 +216,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,79 +253,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -337,103 +391,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -464,9 +464,59 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -490,57 +540,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -549,15 +549,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -570,127 +570,127 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1120,7 +1120,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="5"/>

</xml_diff>